<commit_message>
Added missing OOI Bar codes
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE05MOAS-GL247_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CE05MOAS-GL247_00001.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>Ref Des</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>CC_bsipar_par_scaling</t>
+  </si>
+  <si>
+    <t>OL000359</t>
   </si>
 </sst>
 </file>
@@ -761,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +877,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,9 +1367,11 @@
       <c r="D18" s="9">
         <v>1</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
       <c r="F18" s="14">
-        <v>311</v>
+        <v>247</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>

</xml_diff>